<commit_message>
xbox gamaakt en css file bijgewerkt
</commit_message>
<xml_diff>
--- a/Gannt planning.xlsx
+++ b/Gannt planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/ICT/Opdracht 5 Amo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83E9AFEF-5901-C546-867A-AA20A57BC708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A059BF96-7B96-4642-9983-B3D5DF932AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{7D5636AB-83AB-CE4C-8107-DC27CA58E9DB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{7D5636AB-83AB-CE4C-8107-DC27CA58E9DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Tom</t>
   </si>
   <si>
-    <t>Teamlid 4</t>
-  </si>
-  <si>
     <t>Overleg en Beluistvorming</t>
   </si>
   <si>
@@ -88,13 +85,16 @@
   </si>
   <si>
     <t>Planning Gannt</t>
+  </si>
+  <si>
+    <t>Runa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,8 +102,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +189,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -381,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -406,21 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -448,6 +458,30 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -770,7 +804,7 @@
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -861,65 +895,65 @@
     </row>
     <row r="6" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="16">
+      <c r="B6" s="49">
         <v>43787</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16">
+      <c r="C6" s="50"/>
+      <c r="D6" s="49">
         <v>43788</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16">
+      <c r="E6" s="50"/>
+      <c r="F6" s="49">
         <v>43789</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16">
+      <c r="G6" s="50"/>
+      <c r="H6" s="49">
         <v>43790</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16">
+      <c r="I6" s="50"/>
+      <c r="J6" s="49">
         <v>43791</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16">
+      <c r="K6" s="50"/>
+      <c r="L6" s="49">
         <v>43794</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="16">
+      <c r="M6" s="50"/>
+      <c r="N6" s="49">
         <v>43795</v>
       </c>
-      <c r="O6" s="15"/>
-      <c r="P6" s="16">
+      <c r="O6" s="50"/>
+      <c r="P6" s="49">
         <v>43796</v>
       </c>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="16">
+      <c r="Q6" s="50"/>
+      <c r="R6" s="49">
         <v>43797</v>
       </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="16">
+      <c r="S6" s="50"/>
+      <c r="T6" s="49">
         <v>43798</v>
       </c>
-      <c r="U6" s="15"/>
+      <c r="U6" s="50"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="3"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="19"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="1"/>
@@ -928,21 +962,21 @@
       <c r="U7" s="3"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="4"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="6"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="38"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="4"/>
@@ -951,21 +985,21 @@
       <c r="U8" s="6"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="22"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="27"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="21"/>
+      <c r="I9" s="16"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="6"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="16"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="6"/>
+      <c r="O9" s="16"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="4"/>
@@ -974,13 +1008,13 @@
       <c r="U9" s="6"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="4"/>
       <c r="C10" s="6"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="45"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="44"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="4"/>
       <c r="I10" s="6"/>
       <c r="J10" s="4"/>
@@ -988,7 +1022,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="6"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="6"/>
+      <c r="O10" s="43"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="4"/>
@@ -997,13 +1031,13 @@
       <c r="U10" s="6"/>
     </row>
     <row r="11" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="7"/>
       <c r="C11" s="9"/>
       <c r="D11" s="7"/>
       <c r="E11" s="9"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="7"/>
       <c r="I11" s="9"/>
       <c r="J11" s="7"/>
@@ -1011,7 +1045,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="9"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="9"/>
+      <c r="O11" s="44"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="7"/>
@@ -1020,23 +1054,23 @@
       <c r="U11" s="9"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="3"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="19"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="1"/>
@@ -1045,21 +1079,21 @@
       <c r="U12" s="3"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="4"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="6"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="38"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="4"/>
@@ -1068,21 +1102,21 @@
       <c r="U13" s="6"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="4"/>
       <c r="C14" s="6"/>
       <c r="D14" s="4"/>
       <c r="E14" s="6"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="21"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="21"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="16"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="6"/>
+      <c r="M14" s="16"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="6"/>
+      <c r="O14" s="16"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="4"/>
@@ -1091,21 +1125,21 @@
       <c r="U14" s="6"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
       <c r="E15" s="6"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="44"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="4"/>
       <c r="K15" s="6"/>
       <c r="L15" s="4"/>
       <c r="M15" s="6"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="6"/>
+      <c r="O15" s="43"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="4"/>
@@ -1114,7 +1148,7 @@
       <c r="U15" s="6"/>
     </row>
     <row r="16" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
       <c r="D16" s="7"/>
@@ -1128,7 +1162,7 @@
       <c r="L16" s="7"/>
       <c r="M16" s="9"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="9"/>
+      <c r="O16" s="44"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="7"/>
@@ -1137,23 +1171,23 @@
       <c r="U16" s="9"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="3"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="19"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="1"/>
@@ -1162,21 +1196,21 @@
       <c r="U17" s="3"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="4"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="6"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="38"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="4"/>
@@ -1185,21 +1219,21 @@
       <c r="U18" s="6"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="4"/>
       <c r="C19" s="6"/>
       <c r="D19" s="4"/>
       <c r="E19" s="6"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="21"/>
+      <c r="G19" s="16"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="21"/>
+      <c r="I19" s="16"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="6"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="6"/>
+      <c r="M19" s="16"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="6"/>
+      <c r="O19" s="41"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="4"/>
@@ -1208,21 +1242,21 @@
       <c r="U19" s="6"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="4"/>
       <c r="C20" s="6"/>
       <c r="D20" s="4"/>
       <c r="E20" s="6"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="6"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="4"/>
       <c r="I20" s="6"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="6"/>
+      <c r="K20" s="42"/>
       <c r="L20" s="4"/>
       <c r="M20" s="6"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="6"/>
+      <c r="O20" s="43"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="4"/>
@@ -1231,7 +1265,7 @@
       <c r="U20" s="6"/>
     </row>
     <row r="21" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
       <c r="D21" s="7"/>
@@ -1245,7 +1279,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="9"/>
       <c r="N21" s="7"/>
-      <c r="O21" s="9"/>
+      <c r="O21" s="44"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="7"/>
@@ -1254,55 +1288,55 @@
       <c r="U21" s="9"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>6</v>
+      <c r="A22" s="51" t="s">
+        <v>18</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="6"/>
       <c r="D22" s="4"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="6"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="17"/>
       <c r="R22" s="4"/>
       <c r="S22" s="6"/>
       <c r="T22" s="5"/>
       <c r="U22" s="6"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
+      <c r="A23" s="52"/>
       <c r="B23" s="4"/>
       <c r="C23" s="6"/>
       <c r="D23" s="4"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="6"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="17"/>
       <c r="R23" s="4"/>
       <c r="S23" s="6"/>
       <c r="T23" s="5"/>
       <c r="U23" s="6"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="4"/>
       <c r="C24" s="6"/>
       <c r="D24" s="4"/>
@@ -1310,22 +1344,22 @@
       <c r="F24" s="4"/>
       <c r="G24" s="6"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="6"/>
+      <c r="I24" s="54"/>
       <c r="J24" s="4"/>
       <c r="K24" s="6"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="6"/>
+      <c r="M24" s="42"/>
       <c r="N24" s="4"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="6"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="17"/>
       <c r="R24" s="4"/>
       <c r="S24" s="6"/>
       <c r="T24" s="5"/>
       <c r="U24" s="6"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
+      <c r="A25" s="52"/>
       <c r="B25" s="4"/>
       <c r="C25" s="6"/>
       <c r="D25" s="4"/>
@@ -1340,15 +1374,15 @@
       <c r="M25" s="6"/>
       <c r="N25" s="4"/>
       <c r="O25" s="6"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="6"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="17"/>
       <c r="R25" s="4"/>
       <c r="S25" s="6"/>
       <c r="T25" s="5"/>
       <c r="U25" s="6"/>
     </row>
     <row r="26" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="7"/>
       <c r="C26" s="9"/>
       <c r="D26" s="7"/>
@@ -1375,9 +1409,9 @@
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="28"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="3"/>
@@ -1386,9 +1420,9 @@
       <c r="B30" s="4">
         <v>2</v>
       </c>
-      <c r="C30" s="29"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="6"/>
@@ -1397,9 +1431,9 @@
       <c r="B31" s="4">
         <v>3</v>
       </c>
-      <c r="C31" s="30"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
@@ -1408,9 +1442,9 @@
       <c r="B32" s="4">
         <v>4</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="39" t="s">
-        <v>10</v>
+      <c r="C32" s="26"/>
+      <c r="D32" s="34" t="s">
+        <v>9</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="6"/>
@@ -1419,9 +1453,9 @@
       <c r="B33" s="4">
         <v>5</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="39" t="s">
-        <v>17</v>
+      <c r="C33" s="27"/>
+      <c r="D33" s="34" t="s">
+        <v>16</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="6"/>
@@ -1430,9 +1464,9 @@
       <c r="B34" s="4">
         <v>6</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="39" t="s">
-        <v>11</v>
+      <c r="C34" s="28"/>
+      <c r="D34" s="34" t="s">
+        <v>10</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6"/>
@@ -1441,9 +1475,9 @@
       <c r="B35" s="4">
         <v>7</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="39" t="s">
-        <v>12</v>
+      <c r="C35" s="29"/>
+      <c r="D35" s="34" t="s">
+        <v>11</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="6"/>
@@ -1452,9 +1486,9 @@
       <c r="B36" s="4">
         <v>8</v>
       </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="39" t="s">
-        <v>13</v>
+      <c r="C36" s="30"/>
+      <c r="D36" s="34" t="s">
+        <v>12</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="6"/>
@@ -1463,9 +1497,9 @@
       <c r="B37" s="4">
         <v>9</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="39" t="s">
-        <v>14</v>
+      <c r="C37" s="31"/>
+      <c r="D37" s="34" t="s">
+        <v>13</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="6"/>
@@ -1474,9 +1508,9 @@
       <c r="B38" s="4">
         <v>10</v>
       </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="39" t="s">
-        <v>15</v>
+      <c r="C38" s="32"/>
+      <c r="D38" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="6"/>
@@ -1485,9 +1519,9 @@
       <c r="B39" s="4">
         <v>11</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="39" t="s">
-        <v>16</v>
+      <c r="C39" s="33"/>
+      <c r="D39" s="34" t="s">
+        <v>15</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="6"/>
@@ -1496,9 +1530,9 @@
       <c r="B40" s="7">
         <v>12</v>
       </c>
-      <c r="C40" s="40"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="9"/>

</xml_diff>